<commit_message>
automated_api_insights is the new automated_api_post_metrics , added functions for demographic data and additional metrics such as website_clicks. removed duplicate function for optimization, will likely need to replace with a better strategy. ig_data_scraper includes get request functions for the new additions, as well as deleted some now obselete functions. Added backup folder for data backups.
</commit_message>
<xml_diff>
--- a/data/cleaned_data/daily_profile_metrics.xlsx
+++ b/data/cleaned_data/daily_profile_metrics.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +58,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,84 +441,487 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>datetime_insights_pulled</t>
+          <t>biography</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>follower_count</t>
+          <t>followers_count</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>follows_count</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>media_count</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>profile_picture_url</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>extraction_datetime</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>extraction_date</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>extraction_year</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>extraction_month</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>extraction_day</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>extraction_time</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45730.48572916666</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ᴛʜᴇ ʟᴏᴄ ɢɪʀʟʏ ᴘʀᴀᴄᴛɪᴄɪɴɢ ᴛʜᴇ ᴀʀᴛ ᴏꜰ ꜰᴀɪʟᴜʀᴇ
+🫶🏽 | authenticity, locs, hobbies ✨
+🪴 | 71 Locs est. on 07.20.23
+💌 | locwithaush@gmail.com</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>2721</v>
+        <v>2743</v>
       </c>
       <c r="C2" t="n">
-        <v>140</v>
+        <v>212</v>
+      </c>
+      <c r="D2" t="n">
+        <v>142</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=REf1r7EQt70Q7kNvgGIaT6F&amp;_nc_oc=AdlDa724AZPUwOu3d8D9-8mVPLkwlGWtMGm7AaI8grxK5TqI5dzrsInyzSsD2ftXay8_8EsysnDvc8Mj4dP5LwBc&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYEF-Er9rbSmkvzqTtS_DhWw2qYsrSRE-Emj1By5-_TkKA&amp;oe=67E3B46E</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-03-21 15:32:39.461267</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>21</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>15:32:39</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45732.81328703704</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ᴛʜᴇ ʟᴏᴄ ɢɪʀʟʏ ᴘʀᴀᴄᴛɪᴄɪɴɢ ᴛʜᴇ ᴀʀᴛ ᴏꜰ ꜰᴀɪʟᴜʀᴇ
+🫶🏽 | authenticity, locs, hobbies ✨
+🪴 | 71 Locs est. on 07.20.23
+💌 | locwithaush@gmail.com</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>2726</v>
+        <v>2747</v>
       </c>
       <c r="C3" t="n">
-        <v>138</v>
+        <v>213</v>
+      </c>
+      <c r="D3" t="n">
+        <v>143</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=REf1r7EQt70Q7kNvgF4wLPg&amp;_nc_oc=AdkSYBucOX6Q3J5j5mIvhvE2Hw5jacNuKrsYfgCulPVn5jVgAwQNnS9F8jEnRVefjlGbK7iqNv7A8zhQ4INOzDi3&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYHVBipZCsbj-6rKoYHREp4RtPZjBsd94RgEmF5hwgnPXw&amp;oe=67E505EE</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-03-22 15:32:56.543004</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-03-22</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>22</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>15:32:56</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45733.81351851852</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>🪴 | 71 ʟᴏᴄs est. on 07.20.23
+🫶🏽 | sᴇʟғ-ᴍᴀɪɴᴛᴀɪɴᴇᴅ x ᴛᴡᴏ sᴛʀᴀɴᴅ ᴛᴡɪsᴛs
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx
+💌 | locwithaush@gmail.com</t>
+        </is>
       </c>
       <c r="B4" t="n">
-        <v>2726</v>
+        <v>2759</v>
       </c>
       <c r="C4" t="n">
-        <v>138</v>
+        <v>213</v>
+      </c>
+      <c r="D4" t="n">
+        <v>144</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=xaWqAUtJd4oQ7kNvgFQfbl6&amp;_nc_oc=Adny3OUFYGf0JKJDu8olgTKUJse1wqc6zD13xzoMqhZlxo0XUlG5W3Cu-HAOqXhJH13g7wyf0mChQ4kma5QroCgT&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYGa9oWxWlbM26TGRRd_Pun2479FFafXiF3KK9T0jvdu4g&amp;oe=67E7A8EE</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>45740.76691777778</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-03-24</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>24</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>18:24:21</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45734.81371527778</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>🪴 | 71 ʟᴏᴄs est. on 07.20.23
+🫶🏽 | sᴇʟғ-ᴍᴀɪɴᴛᴀɪɴᴇᴅ x ᴛᴡᴏ sᴛʀᴀɴᴅ ᴛᴡɪsᴛs
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx
+💌 | locwithaush@gmail.com</t>
+        </is>
       </c>
       <c r="B5" t="n">
-        <v>2734</v>
+        <v>2770</v>
       </c>
       <c r="C5" t="n">
-        <v>139</v>
+        <v>215</v>
+      </c>
+      <c r="D5" t="n">
+        <v>146</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=UrmgwBr0UUQQ7kNvgFIdAD2&amp;_nc_oc=Adl6YX3cTPPuS_uHG3zSytgL79FzsI1M5_r9hl_zCo02felRE3tGYFGnrhhAbWpk0gzSHIwK6yGVWFOSPnVJB3_0&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYFgG3eLPZ61RyCOV1Ykrv25US1Sa3oMu3X591GAmyZfew&amp;oe=67EBD5AE</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>45743.84596371528</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2025-03-27</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>27</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>20:18:11</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45735.81390046296</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>🪴 | 71 ʟᴏᴄs est. on 07.20.23
+🫶🏽 | sᴇʟғ-ᴍᴀɪɴᴛᴀɪɴᴇᴅ x ᴛᴡᴏ sᴛʀᴀɴᴅ ᴛᴡɪsᴛs
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx
+💌 | locwithaush@gmail.com</t>
+        </is>
       </c>
       <c r="B6" t="n">
-        <v>2738</v>
+        <v>2776</v>
       </c>
       <c r="C6" t="n">
-        <v>140</v>
+        <v>216</v>
+      </c>
+      <c r="D6" t="n">
+        <v>146</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=UrmgwBr0UUQQ7kNvgHfcU4a&amp;_nc_oc=AdlYUD_kJLmKBefHJ75SiVXoPOLmbMDvnDjWnCjjy3jUVLWXJz8KOK9Symq3vnp-QeIWJHpFZhOjFDPC6yRnWSXL&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYHUsfmB9nHGwNcZMYB6c5B0lSWcl-fG1bTtFwtBaOEIeA&amp;oe=67EEB0EE</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>45745.97267832176</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2025-03-29</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>29</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>23:20:39</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>45736.81356481482</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>🪴 | 71 ʟᴏᴄs est. on 07.20.23
+🫶🏽 | sᴇʟғ-ᴍᴀɪɴᴛᴀɪɴᴇᴅ x ᴛᴡᴏ sᴛʀᴀɴᴅ ᴛᴡɪsᴛs
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx
+💌 | locwithaush@gmail.com</t>
+        </is>
       </c>
       <c r="B7" t="n">
-        <v>2742</v>
+        <v>2781</v>
       </c>
       <c r="C7" t="n">
-        <v>141</v>
+        <v>216</v>
+      </c>
+      <c r="D7" t="n">
+        <v>147</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=tfc3FpujEWIQ7kNvgHIHD9N&amp;_nc_oc=AdlJKvOM6W00f_yCrtz_hV-wJN_R3Ca0WSbHXivJURaFTAFRdp8gtY6BmEmKOSpmgxyeUyFUHJ_w_TK42EH9nj_O&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYH45ou3iyIqkGhxJ83vajVuUF39coT3RoG2D66WSnSfJQ&amp;oe=67F0026E</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>45746.9727872338</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2025-03-30</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>30</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>23:20:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>🪴 | 71 ʟᴏᴄs est. on 07.20.23
+🫶🏽 | sᴇʟғ-ᴍᴀɪɴᴛᴀɪɴᴇᴅ x ᴛᴡᴏ sᴛʀᴀɴᴅ ᴛᴡɪsᴛs
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx
+💌 | locwithaush@gmail.com</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2785</v>
+      </c>
+      <c r="C8" t="n">
+        <v>217</v>
+      </c>
+      <c r="D8" t="n">
+        <v>148</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=tfc3FpujEWIQ7kNvgHLRKQc&amp;_nc_oc=AdnwFuk4HrfuXcGZmep6i70TEdQ22sJ5dvnJg7sqHrOpo7SW-m_5zc5hdb54gppau_Bzsto7vLupMNKbK_pjpIRR&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYEMohSadREpBlw_Gu_7-fYhs9P_EtHUzmHLj8jbrqfd9Q&amp;oe=67F153EE</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>45747.97296697916</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>31</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>23:21:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>✦ 𝗹𝗼𝗰𝘀 ✦ 𝘄𝗲𝗹𝗹𝗻𝗲𝘀𝘀 ✦ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✦
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx
+💌 | locwithaush@gmail.com</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2791</v>
+      </c>
+      <c r="C9" t="n">
+        <v>217</v>
+      </c>
+      <c r="D9" t="n">
+        <v>149</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=tfc3FpujEWIQ7kNvgG3Kh80&amp;_nc_oc=AdnCeMNyTSDGapxyorA3__npsPI3f9s20Ocb79oX_gVo_XSsSyyJN6m-dYOfx8dco_c7Ya8E2HB9VtCmN6bwAh89&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYFWcnXeXbs0VABvFVqWL4uVNO6yMylJn0KroJym_YbILg&amp;oe=67F234EE</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>45748.70299835925</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2025-04-01</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>16:52:19</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added images for each post for Tableau Dashboard. Still need to automate deletion of old images.
</commit_message>
<xml_diff>
--- a/data/cleaned_data/daily_profile_metrics.xlsx
+++ b/data/cleaned_data/daily_profile_metrics.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,13 +629,13 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=xaWqAUtJd4oQ7kNvgFQfbl6&amp;_nc_oc=Adny3OUFYGf0JKJDu8olgTKUJse1wqc6zD13xzoMqhZlxo0XUlG5W3Cu-HAOqXhJH13g7wyf0mChQ4kma5QroCgT&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYGa9oWxWlbM26TGRRd_Pun2479FFafXiF3KK9T0jvdu4g&amp;oe=67E7A8EE</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>45740.76691777778</v>
+      <c r="F4" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-03-24 18:24:21.696310</t>
+        </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -682,13 +682,13 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=UrmgwBr0UUQQ7kNvgFIdAD2&amp;_nc_oc=Adl6YX3cTPPuS_uHG3zSytgL79FzsI1M5_r9hl_zCo02felRE3tGYFGnrhhAbWpk0gzSHIwK6yGVWFOSPnVJB3_0&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYFgG3eLPZ61RyCOV1Ykrv25US1Sa3oMu3X591GAmyZfew&amp;oe=67EBD5AE</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>45743.84596371528</v>
+      <c r="F5" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-03-27 20:18:11.265210</t>
+        </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -735,13 +735,13 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=UrmgwBr0UUQQ7kNvgHfcU4a&amp;_nc_oc=AdlYUD_kJLmKBefHJ75SiVXoPOLmbMDvnDjWnCjjy3jUVLWXJz8KOK9Symq3vnp-QeIWJHpFZhOjFDPC6yRnWSXL&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYHUsfmB9nHGwNcZMYB6c5B0lSWcl-fG1bTtFwtBaOEIeA&amp;oe=67EEB0EE</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>45745.97267832176</v>
+      <c r="F6" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-03-29 23:20:39.406798</t>
+        </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -788,13 +788,13 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=tfc3FpujEWIQ7kNvgHIHD9N&amp;_nc_oc=AdlJKvOM6W00f_yCrtz_hV-wJN_R3Ca0WSbHXivJURaFTAFRdp8gtY6BmEmKOSpmgxyeUyFUHJ_w_TK42EH9nj_O&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYH45ou3iyIqkGhxJ83vajVuUF39coT3RoG2D66WSnSfJQ&amp;oe=67F0026E</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="n">
-        <v>45746.9727872338</v>
+      <c r="F7" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025-03-30 23:20:48.817247</t>
+        </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -841,13 +841,13 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=tfc3FpujEWIQ7kNvgHLRKQc&amp;_nc_oc=AdnwFuk4HrfuXcGZmep6i70TEdQ22sJ5dvnJg7sqHrOpo7SW-m_5zc5hdb54gppau_Bzsto7vLupMNKbK_pjpIRR&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYEMohSadREpBlw_Gu_7-fYhs9P_EtHUzmHLj8jbrqfd9Q&amp;oe=67F153EE</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="n">
-        <v>45747.97296697916</v>
+      <c r="F8" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-03-31 23:21:04.347441</t>
+        </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -894,13 +894,13 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=tfc3FpujEWIQ7kNvgG3Kh80&amp;_nc_oc=AdnCeMNyTSDGapxyorA3__npsPI3f9s20Ocb79oX_gVo_XSsSyyJN6m-dYOfx8dco_c7Ya8E2HB9VtCmN6bwAh89&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYFWcnXeXbs0VABvFVqWL4uVNO6yMylJn0KroJym_YbILg&amp;oe=67F234EE</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="n">
-        <v>45748.70299835925</v>
+      <c r="F9" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025-04-01 16:52:19.058239</t>
+        </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -921,6 +921,1278 @@
       <c r="L9" t="inlineStr">
         <is>
           <t>16:52:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>✦ 𝗹𝗼𝗰𝘀 ✦ 𝘄𝗲𝗹𝗹𝗻𝗲𝘀𝘀 ✦ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✦
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx
+💌 | locwithaush@gmail.com</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2788</v>
+      </c>
+      <c r="C10" t="n">
+        <v>217</v>
+      </c>
+      <c r="D10" t="n">
+        <v>150</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://scontent-dfw5-2.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=H-HEt6jMN7cQ7kNvgEGQsvC&amp;_nc_oc=AdlQIcDngGBYtIpYA7bkh8LuJ956yWDq4Bb0Xz_Pt--SsIJQTDyAtEVLl5lQZZ4GecTZ2IS9tAq4Q6lkxM-1Z5m7&amp;_nc_zt=23&amp;_nc_ht=scontent-dfw5-2.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYFmE1IRNH69GmRyBm7IGuerbVvFen2FQtLfq0TRe7gnSw&amp;oe=67F3866E</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-04-02 16:52:40.013681</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2025-04-02</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>2</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>16:52:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>✦ 𝗹𝗼𝗰𝘀 ✦ 𝘄𝗲𝗹𝗹𝗻𝗲𝘀𝘀 ✦ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✦
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx
+💌 | locwithaush@gmail.com</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2791</v>
+      </c>
+      <c r="C11" t="n">
+        <v>217</v>
+      </c>
+      <c r="D11" t="n">
+        <v>150</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://scontent-dfw5-2.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=H-HEt6jMN7cQ7kNvwENBXmQ&amp;_nc_oc=AdlsTEre1A7g9CIU1HCvgv7_rm_Kju4gLryt-BirH1Z-yJb7LabRS5kNTBBrR1oAwEmVKbP2HW7Z1SzFnQEOKKwq&amp;_nc_zt=23&amp;_nc_ht=scontent-dfw5-2.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYHjM7P6pbfKp-h4gxNNzlmHBMmJtXmJjPq1_ewZxp3VZQ&amp;oe=67F4D7EE</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-04-03 16:53:01.376215</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2025-04-03</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>3</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>16:53:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗴𝗵𝘁 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx
+💌 | locwithaush@gmail.com</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2797</v>
+      </c>
+      <c r="C12" t="n">
+        <v>216</v>
+      </c>
+      <c r="D12" t="n">
+        <v>152</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=H-HEt6jMN7cQ7kNvwElLAit&amp;_nc_oc=AdkvA_t8vKb6XR081qMf-w3hqEdn6nTb9c-4T9DJQVU45jMU7wYIX9DmFPzCR32kol6SP9axVVkWxGXYjMqOb7ye&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AYF2w5zFovkm2AdTIm7X86dB9qqpkzjc34pWGEit1DdbBg&amp;oe=67F6296E</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-04-04 16:52:22.718804</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2025-04-04</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>4</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>16:52:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | 𝑖𝑛𝑛𝑒𝑟 𝑐ℎ𝑖𝑙𝑑 𝑎𝑑𝑣𝑜𝑐𝑎𝑡𝑒
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2808</v>
+      </c>
+      <c r="C13" t="n">
+        <v>219</v>
+      </c>
+      <c r="D13" t="n">
+        <v>153</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=keECspd2MG4Q7kNvwHVMQrD&amp;_nc_oc=Adkx5DvGrr7su2Nf-eH2z2Lz08wKZPHLGlLlSlfefYoev1ZaMrJBWpWPepJAxbPZjOqrbP9TuKOUJeDKLp7nUrED&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHgGq8Kyoa7B20hGDUssFHlTubpLzr1yoUrtJHX4ex9Cg&amp;oe=67F93CEE</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-04-07 00:50:29.998578</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2025-04-07</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>7</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>00:50:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2816</v>
+      </c>
+      <c r="C14" t="n">
+        <v>220</v>
+      </c>
+      <c r="D14" t="n">
+        <v>158</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=aTM3PfcoE5cQ7kNvwEU2P51&amp;_nc_oc=AdnhzLX6m4YlWchWD_CF1DComEGdwnPCANl17CkzGVhNsCL5ao0tLx5_RuMj2mKSe5pvdPzp9vxlVL862mls3Fv6&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfGSgCXuFxV6cWTI-nwgbMDSIIwVBWI8GFVQyu0XlAHWeA&amp;oe=67FBA7AE</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-04-08 20:03:49.900666</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2025-04-08</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>8</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>20:03:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2833</v>
+      </c>
+      <c r="C15" t="n">
+        <v>222</v>
+      </c>
+      <c r="D15" t="n">
+        <v>161</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=jRcikR2x5UoQ7kNvwEi8fSQ&amp;_nc_oc=Adms8nM-CyQNSJqGuk0t__3kvmnB7iPNkF1ul_8XgF00_d0pcmDw649lNhsh9OPdE0bHmOIGU9r7GJE_T1Q90OTl&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfG4MV_Y2xSQW96uG6qMp539SpZI1sdR4a-piOF1hdMC_w&amp;oe=67FF2BAE</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-04-11 11:03:02.012559</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2025-04-11</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>11</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>11:03:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2841</v>
+      </c>
+      <c r="C16" t="n">
+        <v>222</v>
+      </c>
+      <c r="D16" t="n">
+        <v>162</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=jRcikR2x5UoQ7kNvwEBRyTu&amp;_nc_oc=AdkdJ-MHn4NPqepeswhCBL480gt4p7vTF7mO3u98AQL7uPn1bnPs1CLOO1QSpWgkvFlznGEFqSYmEgjLFvUMm2z5&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfG3UPxiC3laNWYVPwMtOQvPyXUQ8dXJYcLpUIKiIpQOrw&amp;oe=68007D2E</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2025-04-12 11:02:50.473294</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2025-04-12</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>12</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>11:02:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2852</v>
+      </c>
+      <c r="C17" t="n">
+        <v>222</v>
+      </c>
+      <c r="D17" t="n">
+        <v>163</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=jRcikR2x5UoQ7kNvwEBRyTu&amp;_nc_oc=AdkdJ-MHn4NPqepeswhCBL480gt4p7vTF7mO3u98AQL7uPn1bnPs1CLOO1QSpWgkvFlznGEFqSYmEgjLFvUMm2z5&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfH7spkTHQXONZkCfMII_fWsVIY27VCMZEZtBgmZTsq_BA&amp;oe=6801CEAE</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-04-13 11:02:18.007481</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2025-04-13</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>13</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>11:02:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2855</v>
+      </c>
+      <c r="C18" t="n">
+        <v>222</v>
+      </c>
+      <c r="D18" t="n">
+        <v>164</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=RYd0qaB1w1UQ7kNvwGABJF9&amp;_nc_oc=AdlPIg8UOEWrKWPFEvHqRpeOhe8gHQBHdR45Wjt99lOXS_kbh-OEpBrEzgzgJ-NnnDtcn7ShfdEl0xOUwtQ6LAR7&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfGklIqd8nlTTNLOZE9qVyE7p_KX0BsT4ipwyB1psJ0MoA&amp;oe=6803202E</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-04-14 11:02:45.751306</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2025-04-14</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>14</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>11:02:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2851</v>
+      </c>
+      <c r="C19" t="n">
+        <v>224</v>
+      </c>
+      <c r="D19" t="n">
+        <v>165</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=RYd0qaB1w1UQ7kNvwGTSFBA&amp;_nc_oc=AdnFH6UuR7J54h90SPGdIiHD7R7sFdakB_5MyW6UFe4fBoFDLtdKr8ZWr9AurwK3dEVsZCVk2-jVr_1Ftdmfo9yN&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHpj314dbbaNyIQKL6fYUAKrdhVV-HuaB_4cmNL7t8fZw&amp;oe=680471AE</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>45762.45992217593</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2025-04-15</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>15</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>11:02:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2857</v>
+      </c>
+      <c r="C20" t="n">
+        <v>225</v>
+      </c>
+      <c r="D20" t="n">
+        <v>167</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=RYd0qaB1w1UQ7kNvwFOJALO&amp;_nc_oc=AdmaCb-kgpNBdV82RqeJaYpZSuEPerXSAbiFALQdu1rf72F_lD-1dsLSMs_-ppn1d_OFboDGOTns21OR632dPk9U&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfGfG12WGh8zf39_kw4xAslqvJVP9Hif_8l_4EF97U2Gbg&amp;oe=6805C32E</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>45763.46002614583</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2025-04-16</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>16</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>11:02:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2861</v>
+      </c>
+      <c r="C21" t="n">
+        <v>225</v>
+      </c>
+      <c r="D21" t="n">
+        <v>167</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Q1PwlYQfxIAQ7kNvwE-0L8h&amp;_nc_oc=Adlsikp9RAiod7K9kuuUWb66l5vykEvAtLTz0G8T1ZFlDIkJCFU9RxH9JCcEwWcfp-SPnVQz3fCu0qo9dviByoJ_&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHfmeGXr2QJcc2915QtPT8RMYIKc7xoqs-qVcgHTjl2NA&amp;oe=680714AE</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>45764.46059219907</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2025-04-17</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>17</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>11:03:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2865</v>
+      </c>
+      <c r="C22" t="n">
+        <v>226</v>
+      </c>
+      <c r="D22" t="n">
+        <v>168</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Q1PwlYQfxIAQ7kNvwGcuOtg&amp;_nc_oc=AdncBWRow9UEvlpW9sJA0x86gmLawVhipChPPQSlcnYO4CdEDQv7_j1ReGa_nRP78y9ndmO1_3scTIiTIizfAGdh&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfFJDU3uh-NZMDPVEUgCXGP0HAT7DFAb8dJoChXdlo9jJQ&amp;oe=6808662E</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>45765.46053376157</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2025-04-18</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>18</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>11:03:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+✨ | Fₐᵢₗᵤᵣₑ Cₒₐcₕ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>2871</v>
+      </c>
+      <c r="C23" t="n">
+        <v>226</v>
+      </c>
+      <c r="D23" t="n">
+        <v>169</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Q1PwlYQfxIAQ7kNvwHOB_yW&amp;_nc_oc=Adk1ZQ2ci8oHu8p-80tyIPRtoST1pxpoHBG7yOJKonpHbwsbOf9Qff39HFpfnKHU6AbpEzuQe1Xw83AvMtSin9N4&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfEvP4vm3NfQVz2wQ0ns6ufeqeM3Uviekrb6eP__KNlmiw&amp;oe=6809B7AE</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>45766.4603133912</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2025-04-19</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>19</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>11:02:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2887</v>
+      </c>
+      <c r="C24" t="n">
+        <v>228</v>
+      </c>
+      <c r="D24" t="n">
+        <v>168</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=eqWF18t31ggQ7kNvwHNTkkM&amp;_nc_oc=AdnuPd9vVOReKHEv_Vq9gKjrOxi8DEA_7Ahlfp1Hm50Np8tPMqdVrEPDWAOXX8UjKUz3nE9dl6znJQl5Wv9hyjAj&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHrAlHlMkx09NREs3CUNeQ2CBMgOWIJUbguXeXiqwCrQA&amp;oe=680CCB2E</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>45768.7933908912</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2025-04-21</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>21</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>19:02:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2899</v>
+      </c>
+      <c r="C25" t="n">
+        <v>229</v>
+      </c>
+      <c r="D25" t="n">
+        <v>170</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=5i3I2csq8uEQ7kNvwEKz7Yd&amp;_nc_oc=AdkRxlM2NhmFwZChQ-1RnUDWaqX_vAAmCy-fhfu94Z5keiJh8_SfO4e89iiSPWAqwel-RsdAh1j_aeVvDQsKaJes&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfE7x0LSIsOvY-TiGQvBzNIP9D0Fe2zUoADhrQ1yAnFEBA&amp;oe=680F6E2E</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>45770.7963471875</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2025-04-23</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>23</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>19:06:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2900</v>
+      </c>
+      <c r="C26" t="n">
+        <v>229</v>
+      </c>
+      <c r="D26" t="n">
+        <v>171</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=5i3I2csq8uEQ7kNvwEKz7Yd&amp;_nc_oc=AdkRxlM2NhmFwZChQ-1RnUDWaqX_vAAmCy-fhfu94Z5keiJh8_SfO4e89iiSPWAqwel-RsdAh1j_aeVvDQsKaJes&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHG4diHIh7SU3gjVOu5fkdMttfXSGTzU9jTO2qqkGORfQ&amp;oe=6810BFAE</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>45771.79633731482</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2025-04-24</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>24</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>19:06:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2912</v>
+      </c>
+      <c r="C27" t="n">
+        <v>231</v>
+      </c>
+      <c r="D27" t="n">
+        <v>172</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=5i3I2csq8uEQ7kNvwEd9nit&amp;_nc_oc=AdmNe1DW6nxiUXbe-r79DYo9FCi9MstBagIYW2455H7uXgc3fWF342dH6SMHA8ThixfnA11WE6tXNUo4fVjSGF4i&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfFHDDBhGBMR81TiGCam1ftLilQWf2V6jlpzyBDxdSfN1g&amp;oe=6812112E</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>45772.79676655093</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2025-04-25</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>25</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>19:07:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2916</v>
+      </c>
+      <c r="C28" t="n">
+        <v>232</v>
+      </c>
+      <c r="D28" t="n">
+        <v>173</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Dz02SseckA4Q7kNvwGK4onp&amp;_nc_oc=Adk5bZBxkx5XVNu2nW5PFK9tL6pDx60g7xbNxR-LkfgGj-bRn6XaFOV-9J8LvIHtNVQpylakm6uLBfhKtqWkbh6T&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfG4-d4a6YXunqUtl0kbO8hAEBlGMgzn1srlgQR7iYg4SQ&amp;oe=681362AE</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G28" s="3" t="n">
+        <v>45773.79669516204</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2025-04-26</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>26</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>19:07:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2920</v>
+      </c>
+      <c r="C29" t="n">
+        <v>233</v>
+      </c>
+      <c r="D29" t="n">
+        <v>174</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Dz02SseckA4Q7kNvwF0SWeh&amp;_nc_oc=AdloBVgDfoo_05jlgC74GtM3-OlzHeHmau2AATCGilmtDiR0Vx7wyBGFnhCZsEPl6vT3iQi80dj14jFpnmwo-Uhm&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHDod5xns9gCB4HbPHARzqU95NU17n4wkCbjgrFa0wW4w&amp;oe=6814B42E</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>45774.79626265046</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2025-04-27</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>27</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>19:06:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>2924</v>
+      </c>
+      <c r="C30" t="n">
+        <v>234</v>
+      </c>
+      <c r="D30" t="n">
+        <v>174</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Dz02SseckA4Q7kNvwFVwDiC&amp;_nc_oc=AdkljOA40prPAIhkPVdr6XHgt5nNh13X9uCtyJevaoM8sjoGTnqS1XHiz10YziJOjRmdiOFKlsSR9kfSg4oRXYxn&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfH0CDz3OUKpX4Ut3hBYfZ23g9cQ5ngmClSw6XtYxeSp7w&amp;oe=681605AE</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G30" s="3" t="n">
+        <v>45775.79613978009</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2025-04-28</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>28</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>19:06:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>2932</v>
+      </c>
+      <c r="C31" t="n">
+        <v>237</v>
+      </c>
+      <c r="D31" t="n">
+        <v>175</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=28p1nT6RoOEQ7kNvwG07osv&amp;_nc_oc=AdmOq0dMbzeCVTYkuwGrkKSM7SM6tCqKy8i_i1wNVqWW8TBy2220Wv1ZEyTOvVVe5IAEXdc0NpPUroGJE3eoXrjo&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfGjlaztThhmMaimy2eW9XO81914jAhWEskkcaXzx37jXg&amp;oe=6817572E</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G31" s="3" t="n">
+        <v>45776.79649628473</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2025-04-29</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>29</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>19:06:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2936</v>
+      </c>
+      <c r="C32" t="n">
+        <v>237</v>
+      </c>
+      <c r="D32" t="n">
+        <v>176</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=28p1nT6RoOEQ7kNvwHGZR9P&amp;_nc_oc=AdnwGTSlb6ySVsLjYhJjInyCp2uQZMk7vJ8qwV6r9_HwXNDuo115nPFuHDebqQSeS2WpnWOSoDhb9RBag8G0gX8S&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfFcwSZRbyRhg4LNNX6NYeTxO08mlcc3I0PpV6NSiCcCvA&amp;oe=6818A8AE</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G32" s="3" t="n">
+        <v>45777.79628887732</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>30</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>19:06:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2940</v>
+      </c>
+      <c r="C33" t="n">
+        <v>237</v>
+      </c>
+      <c r="D33" t="n">
+        <v>177</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=IN_GzJ2sEioQ7kNvwEg5sAD&amp;_nc_oc=AdmbXpAWtsQMCdIwbFTEUc4JIrzUeJ9uIJ4C1O82AyJcxE37ZsWHolsvcoPOTNlvUekXXV9pY0xppZrwjtvdwQuG&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfF2KCp5eD5JwgsRqqE5k-h6S6kr-WVqzqPMiZpcYcAfiA&amp;oe=681AA2EE</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>17841461458191255</t>
+        </is>
+      </c>
+      <c r="G33" s="3" t="n">
+        <v>45779.39787231061</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2025-05-02</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>2</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>09:32:56</t>
         </is>
       </c>
     </row>

</xml_diff>